<commit_message>
chore: update data excel, improve selfcitation, add format lengkap details
</commit_message>
<xml_diff>
--- a/media/excel/dict1_abv_fix.xlsx
+++ b/media/excel/dict1_abv_fix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kuliah\skripsi2\teknis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kuliah\skripsi2\Make Excel File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9FFC3D-9E84-4A93-96D5-92CA907C0D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4ABC61-6EF4-481C-889C-3F5204015151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="352">
   <si>
     <t>Annual</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Sensing</t>
   </si>
   <si>
-    <t xml:space="preserve"> Superconductivity</t>
-  </si>
-  <si>
     <t>Processing</t>
   </si>
   <si>
@@ -695,6 +692,390 @@
   </si>
   <si>
     <t>Automation</t>
+  </si>
+  <si>
+    <t>Acad.</t>
+  </si>
+  <si>
+    <t>Academia</t>
+  </si>
+  <si>
+    <t>Advancements</t>
+  </si>
+  <si>
+    <t>Advances</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>Pr.</t>
+  </si>
+  <si>
+    <t>Clinical</t>
+  </si>
+  <si>
+    <t>Clin.</t>
+  </si>
+  <si>
+    <t>Diseases</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Surv.</t>
+  </si>
+  <si>
+    <t>Surveys</t>
+  </si>
+  <si>
+    <t>Technologies</t>
+  </si>
+  <si>
+    <t>Educational</t>
+  </si>
+  <si>
+    <t>Combinatorial</t>
+  </si>
+  <si>
+    <t>Combinatorics</t>
+  </si>
+  <si>
+    <t>Comb.</t>
+  </si>
+  <si>
+    <t>Comparative</t>
+  </si>
+  <si>
+    <t>Comp.</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>Consum.</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Contracept.</t>
+  </si>
+  <si>
+    <t>Contraception</t>
+  </si>
+  <si>
+    <t>Dyn.</t>
+  </si>
+  <si>
+    <t>Dynamics</t>
+  </si>
+  <si>
+    <t>Dynamical</t>
+  </si>
+  <si>
+    <t>Differentiation</t>
+  </si>
+  <si>
+    <t>Differ.</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Differential</t>
+  </si>
+  <si>
+    <t>Learn.</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Ecol.</t>
+  </si>
+  <si>
+    <t>Ecological</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Electr.</t>
+  </si>
+  <si>
+    <t>Mar.</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>Mechanics.</t>
+  </si>
+  <si>
+    <t>Mech.</t>
+  </si>
+  <si>
+    <t>Meteorology</t>
+  </si>
+  <si>
+    <t>Meteorol.</t>
+  </si>
+  <si>
+    <t>Superconductivity</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Sociol.</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>Psychol.</t>
+  </si>
+  <si>
+    <t>Psychological</t>
+  </si>
+  <si>
+    <t>Psychology</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>Radiat.</t>
+  </si>
+  <si>
+    <t>Eff.</t>
+  </si>
+  <si>
+    <t>Effects</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>Meas.</t>
+  </si>
+  <si>
+    <t>Protection </t>
+  </si>
+  <si>
+    <t>Prot.</t>
+  </si>
+  <si>
+    <t>Aquatic</t>
+  </si>
+  <si>
+    <t>Aquat.</t>
+  </si>
+  <si>
+    <t>Aquatics</t>
+  </si>
+  <si>
+    <t>Ecosystem</t>
+  </si>
+  <si>
+    <t>Ecosyst.</t>
+  </si>
+  <si>
+    <t>Ecosystems</t>
+  </si>
+  <si>
+    <t>Stud.</t>
+  </si>
+  <si>
+    <t>Studies</t>
+  </si>
+  <si>
+    <t>Anim.</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Sciences</t>
+  </si>
+  <si>
+    <t>Theoretical</t>
+  </si>
+  <si>
+    <t>Theor.</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>Exp.</t>
+  </si>
+  <si>
+    <t>Botany</t>
+  </si>
+  <si>
+    <t>Bot.</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Pract.</t>
+  </si>
+  <si>
+    <t>Practices</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>Lit.</t>
+  </si>
+  <si>
+    <t>Literatures</t>
+  </si>
+  <si>
+    <t>Artif.</t>
+  </si>
+  <si>
+    <t>Artificial</t>
+  </si>
+  <si>
+    <t>Astr.</t>
+  </si>
+  <si>
+    <t>Astronomical</t>
+  </si>
+  <si>
+    <t>Astronomics</t>
+  </si>
+  <si>
+    <t>Behav.</t>
+  </si>
+  <si>
+    <t>Behavioral</t>
+  </si>
+  <si>
+    <t>Financ.</t>
+  </si>
+  <si>
+    <t>Finances</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Bus.</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Cognition</t>
+  </si>
+  <si>
+    <t>Cell.</t>
+  </si>
+  <si>
+    <t>Cellular</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Concr.</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Prog.</t>
+  </si>
+  <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t>Eur.</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>Coll.</t>
+  </si>
+  <si>
+    <t>Altern.</t>
+  </si>
+  <si>
+    <t>Alternatives</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Graphical</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Neuroscience</t>
+  </si>
+  <si>
+    <t>Cult.</t>
+  </si>
+  <si>
+    <t>Cultural</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Physiology</t>
+  </si>
+  <si>
+    <t>Physiol.</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Reproduction</t>
+  </si>
+  <si>
+    <t>Reprod.</t>
+  </si>
+  <si>
+    <t>Russ.</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Rom.</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>Academica</t>
+  </si>
+  <si>
+    <t>Academy</t>
   </si>
 </sst>
 </file>
@@ -772,7 +1153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -786,15 +1167,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1133,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L205" sqref="L205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1147,259 +1534,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>86</v>
+      <c r="A1" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>87</v>
+      <c r="A2" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>88</v>
+      <c r="A3" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>89</v>
+      <c r="A4" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+      <c r="A6" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>226</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>227</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>96</v>
+        <v>332</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>97</v>
+        <v>331</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>98</v>
+        <v>293</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>167</v>
+      <c r="A15" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
+      <c r="A16" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
+      <c r="A17" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>103</v>
+        <v>284</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>286</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>105</v>
+      <c r="A21" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>106</v>
+      <c r="A22" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>107</v>
+        <v>308</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>109</v>
+        <v>310</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>311</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>223</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>114</v>
+      <c r="A30" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1407,714 +1794,1365 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>119</v>
+      <c r="A35" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>121</v>
+        <v>318</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>122</v>
+      <c r="A39" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>125</v>
+      <c r="A42" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>319</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>128</v>
+        <v>328</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>130</v>
+      <c r="A47" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>131</v>
+      <c r="A48" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>333</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>334</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>135</v>
+      <c r="A52" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>192</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>53</v>
+      <c r="A56" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>224</v>
+      <c r="A57" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>141</v>
+      <c r="A59" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>144</v>
+      <c r="A62" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>145</v>
+        <v>247</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>149</v>
+        <v>339</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>150</v>
+        <v>340</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>151</v>
+      <c r="A69" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>66</v>
+      <c r="A70" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>152</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>155</v>
+        <v>253</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>156</v>
+        <v>254</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>157</v>
+      <c r="A75" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>160</v>
+      <c r="A78" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>161</v>
+      <c r="A79" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>162</v>
+        <v>250</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>163</v>
+        <v>249</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>164</v>
+        <v>259</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>165</v>
+      <c r="A83" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>166</v>
+      <c r="A84" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>161</v>
+      <c r="A85" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>106</v>
+        <v>287</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>141</v>
+        <v>289</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>160</v>
+      <c r="A88" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>130</v>
+      <c r="A89" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>169</v>
+      <c r="A90" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>169</v>
+      <c r="A91" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>172</v>
+      <c r="A92" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>174</v>
+      <c r="A93" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>176</v>
+      <c r="A94" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>177</v>
+      <c r="A95" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>180</v>
+      <c r="A96" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B97" s="6" t="s">
+      <c r="A97" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
+      <c r="B98" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>186</v>
+      <c r="A99" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>187</v>
+      <c r="A100" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>189</v>
+      <c r="A101" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>189</v>
+      <c r="A102" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
-        <v>192</v>
+      <c r="A103" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>161</v>
+        <v>316</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>194</v>
+      <c r="A105" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>196</v>
+      <c r="A106" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>196</v>
+      <c r="A107" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>196</v>
+      <c r="A108" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>200</v>
+      <c r="A109" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>203</v>
+      <c r="A110" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>205</v>
+      <c r="A111" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>207</v>
+      <c r="A112" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="6" t="s">
-        <v>209</v>
+      <c r="A113" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>210</v>
+      <c r="A114" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>213</v>
+        <v>59</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>212</v>
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
+      <c r="B171" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B119" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B121" s="7" t="s">
-        <v>222</v>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B202">
+    <sortCondition ref="A202"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>